<commit_message>
extracting data from excel for a specific test case
</commit_message>
<xml_diff>
--- a/test_excel.xlsx
+++ b/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA Automation\PythonExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BF0386-85DE-4A09-A3CB-04126DDEE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D841E-1238-471A-BD8A-7000DC6C5B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{911483E3-1472-4EF8-97F1-9F9A9ABC0494}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -50,15 +50,9 @@
     <t>firstName</t>
   </si>
   <si>
-    <t>lastName</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>Test3</t>
-  </si>
-  <si>
     <t>Test4</t>
   </si>
   <si>
@@ -86,15 +80,6 @@
     <t>f</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>j</t>
   </si>
   <si>
@@ -120,6 +105,30 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>test_HomePage_FillingForm</t>
+  </si>
+  <si>
+    <t>Abdur Rehman</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -155,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9051B3F8-9D7B-44C2-8D70-4A59B6591BCE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +513,7 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,91 +524,103 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36048</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D7" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple test datasets for single testcase
</commit_message>
<xml_diff>
--- a/test_excel.xlsx
+++ b/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA Automation\PythonExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D841E-1238-471A-BD8A-7000DC6C5B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEBAD08-511B-440D-BB97-9A5DA5EA7D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{911483E3-1472-4EF8-97F1-9F9A9ABC0494}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Test4</t>
-  </si>
-  <si>
     <t>Test5</t>
   </si>
   <si>
@@ -80,15 +77,6 @@
     <t>f</t>
   </si>
   <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -129,6 +117,15 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Jon Doe</t>
+  </si>
+  <si>
+    <t>jon@test.com</t>
+  </si>
+  <si>
+    <t>JONDOE123</t>
   </si>
 </sst>
 </file>
@@ -504,7 +501,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +521,13 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -538,13 +535,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -552,30 +549,30 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="1">
         <v>36048</v>
@@ -583,44 +580,50 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1">
+        <v>36048</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>